<commit_message>
autograde by product id
</commit_message>
<xml_diff>
--- a/autograding_v1.xlsx
+++ b/autograding_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\virtual\auto_grading\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE32671-DC70-45BE-9FE8-0A03ABB789CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE11408E-9949-42B8-9639-F1F7DB9D711A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6A6A63D0-53F8-4436-A39B-2C8951C3AA68}"/>
+    <workbookView xWindow="33015" yWindow="5340" windowWidth="21675" windowHeight="8970" xr2:uid="{6A6A63D0-53F8-4436-A39B-2C8951C3AA68}"/>
   </bookViews>
   <sheets>
     <sheet name="marlipal" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
   <si>
     <t>MARLIPAL 24/20</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>mN/m</t>
+  </si>
+  <si>
+    <t>product_id</t>
   </si>
 </sst>
 </file>
@@ -135,16 +138,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -158,10 +166,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DF015D9C-2E05-4B19-B2F0-27FEA493B23D}" name="Table1" displayName="Table1" ref="A1:K9" totalsRowShown="0">
-  <autoFilter ref="A1:K9" xr:uid="{EA6F6E96-8685-41DE-B2CB-2E9BFEF8CA11}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DF015D9C-2E05-4B19-B2F0-27FEA493B23D}" name="Table1" displayName="Table1" ref="A1:L9" totalsRowShown="0">
+  <autoFilter ref="A1:L9" xr:uid="{EA6F6E96-8685-41DE-B2CB-2E9BFEF8CA11}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{48ED57D1-E831-4B05-96A5-23157F17938C}" name="grade"/>
+    <tableColumn id="12" xr3:uid="{D41ED102-5A82-4A22-9889-6D301E82BD18}" name="product_id" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{5FB1188C-A7BE-42C5-959E-824599527B11}" name="viscosity_at_20deg"/>
     <tableColumn id="3" xr3:uid="{DFBBB1D5-B07B-4603-B4F7-FFF0CA0CB2A3}" name="visco20_uom"/>
     <tableColumn id="4" xr3:uid="{DBB1CEF6-BED4-429B-8609-78CD634188A8}" name="surf_concen_0.01g/l"/>
@@ -474,346 +483,375 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9931893-AB4F-4606-9DB8-558A1B22E02A}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
+        <v>202105040000304</v>
+      </c>
+      <c r="C2">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>27.5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>24</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>31.2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>200</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
+        <v>202105040000305</v>
+      </c>
+      <c r="C3">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>22</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>40.5</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>16</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>174</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
+        <v>202105040000306</v>
+      </c>
+      <c r="C4">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>28.5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>6</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>22</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>47.5</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>16</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>148</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
+        <v>202105040000307</v>
+      </c>
+      <c r="C5">
         <v>43</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>29</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>7.5</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>22</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>52.9</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>16</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>134</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
+        <v>202105040000308</v>
+      </c>
+      <c r="C6">
         <v>48</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>29.5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>24</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>8</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>22</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>57.6</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>16</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>123</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
+        <v>202105040000309</v>
+      </c>
+      <c r="C7">
         <v>57</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>24</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>12</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>22</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>61.3</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>16</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>112</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2">
+        <v>202105040000310</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>33</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>24</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>15</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>22</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>67.099999999999994</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>16</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>94</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2">
+        <v>202105040000311</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>7</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>35.5</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>17</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>22</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>69.2</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>16</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>83</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>